<commit_message>
MyNN(): small change in weight initialization
</commit_message>
<xml_diff>
--- a/MyTimeSeries/Transform_Scale_Check.xlsx
+++ b/MyTimeSeries/Transform_Scale_Check.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13725"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13725" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="17">
   <si>
     <t>double</t>
   </si>
@@ -99,7 +99,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -130,6 +130,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -143,7 +155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -152,6 +164,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,8 +454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,7 +698,7 @@
         <v>-0.77883668461730093</v>
       </c>
       <c r="N10">
-        <f t="shared" ref="N10:N16" si="8">+M10-M9</f>
+        <f t="shared" ref="N10:N14" si="8">+M10-M9</f>
         <v>0.5095986898580811</v>
       </c>
       <c r="O10">
@@ -943,14 +963,263 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13.140625" style="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8"/>
+      <c r="B1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="11">
+        <f t="shared" ref="A2:A14" si="0">+A3-100000000</f>
+        <v>200208010000</v>
+      </c>
+      <c r="B2" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <f t="shared" si="0"/>
+        <v>200308010000</v>
+      </c>
+      <c r="B3">
+        <f>+B2+1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <f t="shared" si="0"/>
+        <v>200408010000</v>
+      </c>
+      <c r="B4">
+        <f>+B3-2</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <f t="shared" si="0"/>
+        <v>200508010000</v>
+      </c>
+      <c r="B5">
+        <f>+B4-1</f>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <f t="shared" si="0"/>
+        <v>200608010000</v>
+      </c>
+      <c r="B6">
+        <f>+B5+3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <f t="shared" si="0"/>
+        <v>200708010000</v>
+      </c>
+      <c r="B7">
+        <f>+B6+1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <f t="shared" si="0"/>
+        <v>200808010000</v>
+      </c>
+      <c r="B8">
+        <f>+B7-2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <f t="shared" si="0"/>
+        <v>200908010000</v>
+      </c>
+      <c r="B9">
+        <f>+B8-1</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <f t="shared" si="0"/>
+        <v>201008010000</v>
+      </c>
+      <c r="B10">
+        <f>+B9+3</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <f t="shared" si="0"/>
+        <v>201108010000</v>
+      </c>
+      <c r="B11">
+        <f>+B10+1</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <f t="shared" si="0"/>
+        <v>201208010000</v>
+      </c>
+      <c r="B12">
+        <f>+B11-2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
+        <f t="shared" si="0"/>
+        <v>201308010000</v>
+      </c>
+      <c r="B13">
+        <f>+B12-1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <f t="shared" si="0"/>
+        <v>201408010000</v>
+      </c>
+      <c r="B14">
+        <f>+B13+3</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
+        <f>+A16-100000000</f>
+        <v>201508010000</v>
+      </c>
+      <c r="B15">
+        <f>+B14+1</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <v>201608010000</v>
+      </c>
+      <c r="B16">
+        <f>+B15-2</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="10">
+        <f>+A16+100000000</f>
+        <v>201708010000</v>
+      </c>
+      <c r="B17" s="6">
+        <f>+B16-1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
+        <f>+A17+100000000</f>
+        <v>201808010000</v>
+      </c>
+      <c r="B18" s="6">
+        <f>+B17+3</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <f>MIN(B3:B18)</f>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22">
+        <f>MAX(B3:B18)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27">
+        <f>(B24-B25)/(B21-B22)</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28">
+        <f>B25-B27*B22</f>
+        <v>-0.33333333333333326</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>